<commit_message>
commit category vs portal login
</commit_message>
<xml_diff>
--- a/docs/sprint 2 - 1003 To 2203/LogTime.xlsx
+++ b/docs/sprint 2 - 1003 To 2203/LogTime.xlsx
@@ -191,8 +191,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:M9" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:M9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:M8" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:M8"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="10/03/2014"/>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
commit category vs login
</commit_message>
<xml_diff>
--- a/docs/sprint 2 - 1003 To 2203/LogTime.xlsx
+++ b/docs/sprint 2 - 1003 To 2203/LogTime.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ANLT" sheetId="1" r:id="rId1"/>
     <sheet name="QUANGD" sheetId="2" r:id="rId2"/>
     <sheet name="ANHDT" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Nhận update từ phía A.Hoàng</t>
   </si>
@@ -110,12 +110,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tài liệu - Danh sách các màn hình sẽ làm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thời gian đã sử dụng </t>
-  </si>
-  <si>
-    <t>Mức độ Busy</t>
   </si>
   <si>
     <t>Mock-up wishlist</t>
@@ -523,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,6 +658,9 @@
       <c r="G6">
         <v>1</v>
       </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -675,7 +672,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M8">
         <v>3</v>
@@ -691,10 +688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A12:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +724,7 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
@@ -821,16 +818,6 @@
       </c>
       <c r="D9">
         <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -881,7 +868,7 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
@@ -904,7 +891,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>4</v>

</xml_diff>